<commit_message>
optimization of adding users
</commit_message>
<xml_diff>
--- a/CollectedData/Collected_info_user.xlsx
+++ b/CollectedData/Collected_info_user.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Имя</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Время создания заявки</t>
   </si>
   <si>
+    <t>Тест</t>
+  </si>
+  <si>
     <t>Денис</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t>Тимур</t>
   </si>
   <si>
+    <t>Тимурчик</t>
+  </si>
+  <si>
     <t>Николаенко</t>
   </si>
   <si>
@@ -70,7 +76,13 @@
     <t>Бессонович</t>
   </si>
   <si>
-    <t>89001074658</t>
+    <t>Мусаевчик</t>
+  </si>
+  <si>
+    <t>89001083247</t>
+  </si>
+  <si>
+    <t>test@mail.ru</t>
   </si>
   <si>
     <t>denis.nikolaenko.2004@mail.ru</t>
@@ -91,7 +103,10 @@
     <t>koluasik@mail.ru</t>
   </si>
   <si>
-    <t>19</t>
+    <t>musaev.timur@mail.ru</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
   <si>
     <t>Студенты</t>
@@ -106,6 +121,9 @@
     <t>Все</t>
   </si>
   <si>
+    <t>24.05.2023 12:55</t>
+  </si>
+  <si>
     <t>24.05.2023 09:25</t>
   </si>
   <si>
@@ -125,6 +143,9 @@
   </si>
   <si>
     <t>24.05.2023 10:58</t>
+  </si>
+  <si>
+    <t>24.05.2023 11:57</t>
   </si>
 </sst>
 </file>
@@ -482,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -516,22 +537,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>89001083249</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -539,22 +560,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>89001083247</v>
+        <v>89001083249</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -562,22 +583,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>89134053973</v>
+        <v>89001083247</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E4">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -585,22 +606,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>89001256478</v>
+        <v>89134053973</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E5">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -608,45 +629,45 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>89001083249</v>
+        <v>89001256478</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E6">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>89001083249</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -654,22 +675,68 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>89001083249</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
       <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>89001074658</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>89521656455</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="G8" t="s">
-        <v>36</v>
+      <c r="E10">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xz chto sdelal, zabыl
</commit_message>
<xml_diff>
--- a/CollectedData/Collected_info_user.xlsx
+++ b/CollectedData/Collected_info_user.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
   <si>
     <t>Имя</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Время создания заявки</t>
   </si>
   <si>
+    <t>Олег</t>
+  </si>
+  <si>
     <t>Абоба</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t>Тимурчик</t>
   </si>
   <si>
+    <t>Бажайкин</t>
+  </si>
+  <si>
     <t>Абобович</t>
   </si>
   <si>
@@ -100,7 +106,10 @@
     <t>Мусаевчик</t>
   </si>
   <si>
-    <t>89001083249</t>
+    <t>79521656455</t>
+  </si>
+  <si>
+    <t>bashay.oleg@mail.ru</t>
   </si>
   <si>
     <t>aboba@mail.ru</t>
@@ -139,7 +148,7 @@
     <t>musaev.timur@mail.ru</t>
   </si>
   <si>
-    <t>19</t>
+    <t>21</t>
   </si>
   <si>
     <t>Студенты</t>
@@ -152,6 +161,9 @@
   </si>
   <si>
     <t>Учащиеся общеобразоветельных учреждение 8-11 классы</t>
+  </si>
+  <si>
+    <t>01.06.2023 11:31</t>
   </si>
   <si>
     <t>25.05.2023 12:46</t>
@@ -548,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -582,22 +594,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -605,22 +617,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>89001083249</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -628,22 +640,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>89531701180</v>
+        <v>89001083249</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -651,22 +663,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5">
-        <v>89001083249</v>
+        <v>89531701180</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -674,22 +686,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C6">
-        <v>89001083247</v>
+        <v>89001083249</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -697,22 +709,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>89001083249</v>
+        <v>89001083247</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -720,22 +732,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>89001083247</v>
+        <v>89001083249</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E8">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -743,91 +755,91 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9">
-        <v>89134053973</v>
+        <v>89001083247</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
         <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>89001256478</v>
+        <v>89134053973</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E10">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11">
-        <v>89001083249</v>
+        <v>89001256478</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>89001083249</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E12">
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -835,45 +847,68 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>89001074658</v>
+        <v>89001083249</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14">
-        <v>89521656455</v>
+        <v>89001074658</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E14">
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>89521656455</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>